<commit_message>
#comment minor corrections on review document and bug fix on S/UTP - S/STP totals
</commit_message>
<xml_diff>
--- a/doc/sprint1/1121224/Building 2.xlsx
+++ b/doc/sprint1/1121224/Building 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao_\OneDrive\Documentos\rcomp_g03\doc\sprint1\1121224\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FC45C7-D472-4B4D-8FFF-A524C2F4355A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D062D53F-23FB-45DD-9028-89C412F61D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8E827E23-E974-4404-9000-91DF8D0EBF74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E827E23-E974-4404-9000-91DF8D0EBF74}"/>
   </bookViews>
   <sheets>
     <sheet name="Building 2" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="135">
   <si>
     <t xml:space="preserve">2x patch cord fiber </t>
   </si>
@@ -1030,7 +1030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0854720-448F-4157-BD2C-35D09E8B5586}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -1425,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7914A4B8-CE2C-4454-97EE-10F1E320B580}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,9 +1648,6 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="B16" s="10" t="s">
         <v>21</v>
       </c>
@@ -1661,10 +1658,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>70</v>
-      </c>
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
         <v>104</v>
       </c>
@@ -1675,7 +1669,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="7" t="s">
         <v>121</v>
       </c>
@@ -1683,7 +1677,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="11" t="s">
         <v>16</v>
       </c>
@@ -1691,7 +1685,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="9" t="s">
         <v>97</v>
       </c>
@@ -1699,7 +1693,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="10" t="s">
         <v>21</v>
       </c>
@@ -1707,7 +1701,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="8" t="s">
         <v>122</v>
       </c>
@@ -1715,52 +1709,52 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D25" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D27" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="8" t="s">
         <v>96</v>
       </c>

</xml_diff>